<commit_message>
dodano skrypty na przywrócenie identity na ID
</commit_message>
<xml_diff>
--- a/Pytania do Promotora.xlsx
+++ b/Pytania do Promotora.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zbyszard v.2\Desktop\inzynier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7297EB-1D9F-4680-8280-78E0FF6E25AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1942A14F-ED45-43D9-9288-35DED4CD1808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
+    <workbookView xWindow="32955" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,33 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Potworzyć gotowe zbiory call’i w PostManie</t>
   </si>
   <si>
-    <t>Opanować większą ilość błedów</t>
-  </si>
-  <si>
     <t>Potestować wszystkie endpointy na wszelkie sposoby</t>
   </si>
   <si>
-    <t>Dopisać ciekawsze selecty w gui i api</t>
-  </si>
-  <si>
-    <t>autoincrement po wykonianiu populacji</t>
-  </si>
-  <si>
-    <t>CURRENTLY</t>
-  </si>
-  <si>
     <t>TO_DO</t>
   </si>
   <si>
     <t xml:space="preserve">podzielić na pliki </t>
-  </si>
-  <si>
-    <t>Statusy w return</t>
   </si>
   <si>
     <t>Swagger</t>
@@ -454,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E66B81-FB29-4C52-8B6D-AE386FFB343D}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F4" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +452,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -482,42 +467,16 @@
     </row>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
poprawiono update, czytelnosc zapytan sql
</commit_message>
<xml_diff>
--- a/Pytania do Promotora.xlsx
+++ b/Pytania do Promotora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zbyszard v.2\Desktop\inzynier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1942A14F-ED45-43D9-9288-35DED4CD1808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AB457E-849D-4EAB-A0AE-FA1BE6A4F927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32955" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Potworzyć gotowe zbiory call’i w PostManie</t>
   </si>
   <si>
-    <t>Potestować wszystkie endpointy na wszelkie sposoby</t>
-  </si>
-  <si>
     <t>TO_DO</t>
   </si>
   <si>
@@ -51,6 +48,15 @@
   </si>
   <si>
     <t>Inżynierka</t>
+  </si>
+  <si>
+    <t>TO_ASK</t>
+  </si>
+  <si>
+    <t>GminaRelacja - zmienić na EFF_DT?</t>
+  </si>
+  <si>
+    <t>Z powodu GminaRelacja update kolumny start_date który jest jednocześnie kluczem główny zaczyna wywalać z powodu tabeli GminaRelacja</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E66B81-FB29-4C52-8B6D-AE386FFB343D}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F3:F4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,33 +458,50 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
zmieniono baze danych i dodano triggery zamiast fk
</commit_message>
<xml_diff>
--- a/Pytania do Promotora.xlsx
+++ b/Pytania do Promotora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zbyszard v.2\Desktop\inzynier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AB457E-849D-4EAB-A0AE-FA1BE6A4F927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B42FBBA-8D3A-4D65-BB03-1DACEBDE83CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32955" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Potworzyć gotowe zbiory call’i w PostManie</t>
   </si>
@@ -47,16 +47,7 @@
     <t>Swagger</t>
   </si>
   <si>
-    <t>Inżynierka</t>
-  </si>
-  <si>
-    <t>TO_ASK</t>
-  </si>
-  <si>
-    <t>GminaRelacja - zmienić na EFF_DT?</t>
-  </si>
-  <si>
-    <t>Z powodu GminaRelacja update kolumny start_date który jest jednocześnie kluczem główny zaczyna wywalać z powodu tabeli GminaRelacja</t>
+    <t>Inżynierka (opisac dane, potem model, znowu dane, i tabele GminaRelacja i jej triggery i czemu triggery)</t>
   </si>
 </sst>
 </file>
@@ -445,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E66B81-FB29-4C52-8B6D-AE386FFB343D}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -481,28 +472,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ostatnie zmiany, propozycje zmian na jutro, dodane kolejne requesty do postmana
</commit_message>
<xml_diff>
--- a/Pytania do Promotora.xlsx
+++ b/Pytania do Promotora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zbyszard v.2\Desktop\inzynier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B42FBBA-8D3A-4D65-BB03-1DACEBDE83CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0108D1F4-0480-4E7C-B925-BF138FD9148C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32955" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Potworzyć gotowe zbiory call’i w PostManie</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Inżynierka (opisac dane, potem model, znowu dane, i tabele GminaRelacja i jej triggery i czemu triggery)</t>
+  </si>
+  <si>
+    <t>TO_ASK</t>
+  </si>
+  <si>
+    <t>Czy pasowałoby utworzyć partycje na tabelach głównych oraz relacyjnych na poszczególne okresy czasowe? Czasy zapytań i operacji powinny ulec poprawie</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E66B81-FB29-4C52-8B6D-AE386FFB343D}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +478,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
poprawiony insert, poniewaz przestał działac po usunieciu zbednych ustawien
</commit_message>
<xml_diff>
--- a/Pytania do Promotora.xlsx
+++ b/Pytania do Promotora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zbyszard v.2\Desktop\inzynier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0108D1F4-0480-4E7C-B925-BF138FD9148C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8607A2-214C-42C1-8187-E9E292147244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32955" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11C69576-D033-451C-B68A-71E4F35EE0CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Potworzyć gotowe zbiory call’i w PostManie</t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">podzielić na pliki </t>
   </si>
   <si>
-    <t>Swagger</t>
-  </si>
-  <si>
     <t>Inżynierka (opisac dane, potem model, znowu dane, i tabele GminaRelacja i jej triggery i czemu triggery)</t>
   </si>
   <si>
@@ -54,6 +51,12 @@
   </si>
   <si>
     <t>Czy pasowałoby utworzyć partycje na tabelach głównych oraz relacyjnych na poszczególne okresy czasowe? Czasy zapytań i operacji powinny ulec poprawie</t>
+  </si>
+  <si>
+    <t>wspomnieć o case sensitivity endpointów w inżynierce</t>
+  </si>
+  <si>
+    <t>wspomniec o niedzialajacym werkzeugu</t>
   </si>
 </sst>
 </file>
@@ -442,15 +445,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E66B81-FB29-4C52-8B6D-AE386FFB343D}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="49.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -465,28 +468,33 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>